<commit_message>
Final Assignment 6 Submission
</commit_message>
<xml_diff>
--- a/questions/Assignment6-ClientCommandTableForA7.xlsx
+++ b/questions/Assignment6-ClientCommandTableForA7.xlsx
@@ -443,15 +443,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
@@ -462,6 +453,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,6 +537,136 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>103909</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3133725</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>25978</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1943100" y="11543434"/>
+          <a:ext cx="8039100" cy="4894119"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3374129" cy="471860"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4000500" y="11172825"/>
+          <a:ext cx="3374129" cy="471860"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:miter lim="400000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="none"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="3200" b="1" i="1" u="sng" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+              <a:sym typeface="Helvetica Neue"/>
+            </a:rPr>
+            <a:t>STATE MACHINE</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1619,8 +1749,8 @@
   </sheetPr>
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="13.5" customHeight="1"/>
@@ -1637,13 +1767,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="14.65" customHeight="1">
       <c r="A1" s="2"/>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26"/>
     </row>
     <row r="2" spans="1:6" ht="12" customHeight="1">
       <c r="A2" s="3"/>
@@ -1716,7 +1846,7 @@
       <c r="B7" s="8"/>
       <c r="C7" s="9"/>
       <c r="D7" s="10"/>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="20" t="s">
         <v>41</v>
       </c>
       <c r="F7" s="12"/>
@@ -1787,10 +1917,10 @@
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="16"/>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="22" t="s">
         <v>44</v>
       </c>
       <c r="F14" s="16"/>
@@ -1809,10 +1939,10 @@
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="16"/>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="22" t="s">
         <v>43</v>
       </c>
       <c r="F16" s="16"/>
@@ -1866,7 +1996,7 @@
       <c r="B21" s="17"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
-      <c r="E21" s="23" t="s">
+      <c r="E21" s="20" t="s">
         <v>37</v>
       </c>
       <c r="F21" s="16"/>
@@ -1876,18 +2006,18 @@
       <c r="B22" s="4"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
-      <c r="E22" s="24" t="s">
+      <c r="E22" s="21" t="s">
         <v>38</v>
       </c>
       <c r="F22" s="16"/>
     </row>
     <row r="23" spans="1:6" ht="39.75" customHeight="1">
       <c r="A23" s="4"/>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="23" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="16"/>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="22" t="s">
         <v>40</v>
       </c>
       <c r="E23" s="18" t="s">
@@ -1902,7 +2032,7 @@
       <c r="B24" s="17"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
-      <c r="E24" s="23" t="s">
+      <c r="E24" s="20" t="s">
         <v>45</v>
       </c>
       <c r="F24" s="19"/>
@@ -1911,10 +2041,10 @@
       <c r="A25" s="4"/>
       <c r="B25" s="17"/>
       <c r="C25" s="16"/>
-      <c r="D25" s="25" t="s">
+      <c r="D25" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="E25" s="23" t="s">
+      <c r="E25" s="20" t="s">
         <v>37</v>
       </c>
       <c r="F25" s="19"/>
@@ -1923,8 +2053,8 @@
       <c r="A26" s="4"/>
       <c r="B26" s="17"/>
       <c r="C26" s="16"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="23" t="s">
+      <c r="D26" s="22"/>
+      <c r="E26" s="20" t="s">
         <v>42</v>
       </c>
       <c r="F26" s="19"/>
@@ -1933,10 +2063,10 @@
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="16"/>
-      <c r="D27" s="25" t="s">
+      <c r="D27" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="E27" s="25" t="s">
+      <c r="E27" s="22" t="s">
         <v>46</v>
       </c>
       <c r="F27" s="16"/>
@@ -1998,7 +2128,7 @@
       <c r="B33" s="4"/>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
-      <c r="E33" s="25" t="s">
+      <c r="E33" s="22" t="s">
         <v>39</v>
       </c>
       <c r="F33" s="16"/>
@@ -2020,5 +2150,6 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>